<commit_message>
Added use case descriptions
</commit_message>
<xml_diff>
--- a/workspace/Progress.xlsx
+++ b/workspace/Progress.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Things to be done</t>
   </si>
@@ -490,7 +490,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -652,6 +652,9 @@
       <c r="A13" t="s">
         <v>31</v>
       </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -659,6 +662,12 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">

</xml_diff>